<commit_message>
insersao de features dom freq
</commit_message>
<xml_diff>
--- a/Features_inicias.xlsx
+++ b/Features_inicias.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniela\Dropbox\UFOP-2024-1\PDSE\pesquisa\shape-based_Statistics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniela\Documents\daniela\cod\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,16 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="54">
-  <si>
-    <t>Tamanho</t>
-  </si>
-  <si>
-    <t>Forma</t>
-  </si>
-  <si>
-    <t>Relação N/C</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="53">
   <si>
     <t>area</t>
   </si>
@@ -42,9 +33,6 @@
     <t>eccentricity</t>
   </si>
   <si>
-    <t>Borda</t>
-  </si>
-  <si>
     <t>extent (area/BB_area)</t>
   </si>
   <si>
@@ -67,9 +55,6 @@
   </si>
   <si>
     <t>perimeter</t>
-  </si>
-  <si>
-    <t>solidity (area/convexhull_area</t>
   </si>
   <si>
     <t>equivalent_diameter (circle)</t>
@@ -175,12 +160,6 @@
     <t>area_NC</t>
   </si>
   <si>
-    <t>Features extraídas 2 vezes (para nucleo e cito)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Features N/C </t>
-  </si>
-  <si>
     <t>Total:  49</t>
   </si>
   <si>
@@ -188,6 +167,24 @@
   </si>
   <si>
     <t>s</t>
+  </si>
+  <si>
+    <t>Extracted Features - nucleus e cytoplasm</t>
+  </si>
+  <si>
+    <t>Descriptors  N/C</t>
+  </si>
+  <si>
+    <t>Border</t>
+  </si>
+  <si>
+    <t>Shape</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Size</t>
+  </si>
+  <si>
+    <t>solidity (area/convexhull_area)</t>
   </si>
 </sst>
 </file>
@@ -197,7 +194,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000000000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -235,6 +232,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="17"/>
+      <color rgb="FF2AA198"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -250,7 +254,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -317,11 +321,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -331,30 +355,56 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -636,248 +686,248 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E28"/>
+  <dimension ref="B2:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="74.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="74.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="20" t="s">
+    <row r="2" spans="2:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="B2" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="E3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="C4" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="F4" s="15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="22"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="22"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="22"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="9" t="s">
+      <c r="C11" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="8"/>
+      <c r="C12" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="7"/>
+      <c r="C13" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="9"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="14" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="11" t="s">
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="12" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="9"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="9"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="12"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="18" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="B16" s="2"/>
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="B17" s="2"/>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="B19" s="2"/>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="B20" s="2"/>
-    </row>
-    <row r="21" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="B21" s="2"/>
-    </row>
-    <row r="22" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="B22" s="2"/>
-    </row>
-    <row r="23" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="B23" s="2"/>
-    </row>
-    <row r="24" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="B24" s="2"/>
-    </row>
-    <row r="25" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="B25" s="2"/>
-    </row>
-    <row r="26" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A26" t="e">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="2:6" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="C17" s="2"/>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="2:6" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="C18" s="27"/>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="2:6" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="C20" s="2"/>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="2:6" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="C21" s="2"/>
+    </row>
+    <row r="22" spans="2:6" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="C22" s="2"/>
+    </row>
+    <row r="23" spans="2:6" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="C23" s="2"/>
+    </row>
+    <row r="24" spans="2:6" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="C24" s="2"/>
+    </row>
+    <row r="25" spans="2:6" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="C25" s="2"/>
+    </row>
+    <row r="26" spans="2:6" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="C26" s="2"/>
+    </row>
+    <row r="27" spans="2:6" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="B27" t="e">
         <f>#REF!*LOG(#REF!,2)</f>
         <v>#REF!</v>
       </c>
-      <c r="B26" s="2"/>
-    </row>
-    <row r="27" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A27" t="e">
+      <c r="C27" s="2"/>
+    </row>
+    <row r="28" spans="2:6" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="B28" t="e">
         <f>#REF!*LOG(#REF!,2)</f>
         <v>#REF!</v>
       </c>
-      <c r="B27" s="2"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="e">
-        <f>SUM(A26:A27)</f>
+      <c r="C28" s="2"/>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" t="e">
+        <f>SUM(B27:B28)</f>
         <v>#REF!</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A13:D13"/>
+  <mergeCells count="4">
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="D4:D7"/>
+    <mergeCell ref="E4:E7"/>
+    <mergeCell ref="B2:F2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -894,183 +944,183 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="8" t="s">
+      <c r="L1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="N1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="O1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="P1" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" s="8" t="s">
+      <c r="Q1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="R1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="S1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="T1" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="U1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="P1" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q1" s="8" t="s">
+      <c r="V1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="W1" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="X1" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="Y1" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="Z1" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="AA1" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="U1" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="V1" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="W1" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="X1" s="8" t="s">
+      <c r="AC1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="Y1" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z1" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA1" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="AB1" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="AC1" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="AD1" s="8"/>
+      <c r="AD1" s="6"/>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="AA2" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="AD2" s="3"/>
     </row>

</xml_diff>